<commit_message>
Deployed 21ffaa8 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E43">

</xml_diff>

<commit_message>
Deployed 081031e with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E43">
@@ -1876,22 +1876,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E55">
@@ -1904,22 +1904,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E56">

</xml_diff>

<commit_message>
Deployed 9429c67 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E43">

</xml_diff>

<commit_message>
Deployed f8fa837 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>unassigned</t>
         </is>
       </c>
       <c r="E43">

</xml_diff>

<commit_message>
Deployed 2f2b578 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1153,17 +1153,17 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E29">
@@ -1489,17 +1489,17 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E41">
@@ -1512,22 +1512,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>307c55294ffe3b8aa46fce358d55590e</t>
+          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E42">
@@ -1540,22 +1540,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>c0a3f3ed23f04247d92740a9502f8b57</t>
+          <t>307c55294ffe3b8aa46fce358d55590e</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E43">
@@ -1876,22 +1876,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5e733a21f67e541f28ed4bf4fe025044</t>
+          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E55">
@@ -1904,22 +1904,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>975b1dbdc7405f6e27bf63893e91e0ed</t>
+          <t>5e733a21f67e541f28ed4bf4fe025044</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E56">
@@ -2021,17 +2021,17 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>unassigned</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E60">

</xml_diff>

<commit_message>
Deployed 904bad3 with MkDocs version: 1.6.1
</commit_message>
<xml_diff>
--- a/eDNA/example_output/ASV_breakdown.xlsx
+++ b/eDNA/example_output/ASV_breakdown.xlsx
@@ -1074,7 +1074,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Pig</t>
+          <t>Wild boar</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -8008,7 +8008,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>01e4409abad7810cb9232bf5c3bf3d47</t>
+          <t>4450a6fa10b56881617cff33c5585aa8</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -8036,7 +8036,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>4450a6fa10b56881617cff33c5585aa8</t>
+          <t>01e4409abad7810cb9232bf5c3bf3d47</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -9212,22 +9212,22 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>f1836eba7b45e524d0dd854d16773b8e</t>
+          <t>86df320d5c069bed174ca25ba453aac6</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E317">
@@ -9240,22 +9240,22 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>86df320d5c069bed174ca25ba453aac6</t>
+          <t>f1836eba7b45e524d0dd854d16773b8e</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E318">
@@ -10080,17 +10080,17 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>0d64b13f3f45a49980306fedfd13c311</t>
+          <t>060ba27b56f58c034440c81a8ed55f51</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
@@ -10108,17 +10108,17 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>060ba27b56f58c034440c81a8ed55f51</t>
+          <t>0d64b13f3f45a49980306fedfd13c311</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -10696,22 +10696,22 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>98dd82f2d86d0cc318518bed186b2e08</t>
+          <t>454135396336cd1eba14bb5453af6b9e</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E370">
@@ -10724,22 +10724,22 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>454135396336cd1eba14bb5453af6b9e</t>
+          <t>98dd82f2d86d0cc318518bed186b2e08</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E371">
@@ -10948,7 +10948,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>72f3ca241362b9e8bf3c8fec8fcc32ff</t>
+          <t>1dd0f1ca2adf649d8cba813ea6e43de2</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -10976,7 +10976,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>1dd0f1ca2adf649d8cba813ea6e43de2</t>
+          <t>72f3ca241362b9e8bf3c8fec8fcc32ff</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -11312,22 +11312,22 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>825810711e50f4a04d8f97b1ffe93eed</t>
+          <t>0ffdd429f2bc2c852745fef5d7de920c</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
         <is>
-          <t>Larus delawarensis</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>Ring billed gull</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E392">
@@ -11340,22 +11340,22 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>0ffdd429f2bc2c852745fef5d7de920c</t>
+          <t>825810711e50f4a04d8f97b1ffe93eed</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Larus delawarensis</t>
         </is>
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Ring billed gull</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E393">
@@ -12572,22 +12572,22 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>2139fe705bf4d2f50f367444733dfb1c</t>
+          <t>b018de6baa2487f526a381b19a607386</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>Delphinus delphis</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>Shortbeaked common dolphin</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
         <is>
-          <t>Marine Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E437">
@@ -12600,22 +12600,22 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>b018de6baa2487f526a381b19a607386</t>
+          <t>2139fe705bf4d2f50f367444733dfb1c</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Delphinus delphis</t>
         </is>
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Shortbeaked common dolphin</t>
         </is>
       </c>
       <c r="D438" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Marine Mammal</t>
         </is>
       </c>
       <c r="E438">
@@ -12740,22 +12740,22 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>2073247497364fcac26babc83f4c329d</t>
+          <t>20c2df8130fc365b7f334f730552eb9c</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
         <is>
-          <t>Pomatomus saltatrix</t>
+          <t>Anas sp</t>
         </is>
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>Bluefish</t>
+          <t>Mallard sp</t>
         </is>
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E443">
@@ -12768,22 +12768,22 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>20c2df8130fc365b7f334f730552eb9c</t>
+          <t>2073247497364fcac26babc83f4c329d</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
         <is>
-          <t>Anas sp</t>
+          <t>Pomatomus saltatrix</t>
         </is>
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>Mallard sp</t>
+          <t>Bluefish</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E444">
@@ -13944,17 +13944,17 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>0cf545c6b6ec03c1c9b5b78efc9e248e</t>
+          <t>51ba651e66f3c6568db5aa853d7e4e62</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D486" t="inlineStr">
@@ -13972,17 +13972,17 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>51ba651e66f3c6568db5aa853d7e4e62</t>
+          <t>0cf545c6b6ec03c1c9b5b78efc9e248e</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D487" t="inlineStr">
@@ -14000,22 +14000,22 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>95e7ebc184132a4c051f78e3eeee47c6</t>
+          <t>8493cc790a25f38fd47548a6aefb6a7a</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E488">
@@ -14028,22 +14028,22 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>8493cc790a25f38fd47548a6aefb6a7a</t>
+          <t>95e7ebc184132a4c051f78e3eeee47c6</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D489" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E489">
@@ -14168,17 +14168,17 @@
     <row r="494">
       <c r="A494" t="inlineStr">
         <is>
-          <t>f5d92935dd2772c26228ba4531eac8ea</t>
+          <t>c8c661fc76a5c7cdf7e094685344c568</t>
         </is>
       </c>
       <c r="B494" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
@@ -14196,17 +14196,17 @@
     <row r="495">
       <c r="A495" t="inlineStr">
         <is>
-          <t>c8c661fc76a5c7cdf7e094685344c568</t>
+          <t>f5d92935dd2772c26228ba4531eac8ea</t>
         </is>
       </c>
       <c r="B495" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C495" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D495" t="inlineStr">
@@ -14476,22 +14476,22 @@
     <row r="505">
       <c r="A505" t="inlineStr">
         <is>
-          <t>76d87af44706817adcf635b427d64983</t>
+          <t>8057c8d0f0c8a3d2c958da0fec6530d4</t>
         </is>
       </c>
       <c r="B505" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E505">
@@ -14504,22 +14504,22 @@
     <row r="506">
       <c r="A506" t="inlineStr">
         <is>
-          <t>8057c8d0f0c8a3d2c958da0fec6530d4</t>
+          <t>76d87af44706817adcf635b427d64983</t>
         </is>
       </c>
       <c r="B506" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E506">
@@ -14616,22 +14616,22 @@
     <row r="510">
       <c r="A510" t="inlineStr">
         <is>
-          <t>5301bbc32276ce7d3caf98531cc72308</t>
+          <t>789c3558c73ed5654b562b424681009a</t>
         </is>
       </c>
       <c r="B510" t="inlineStr">
         <is>
-          <t>Merluccius bilinearis</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>Silver hake</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E510">
@@ -14644,22 +14644,22 @@
     <row r="511">
       <c r="A511" t="inlineStr">
         <is>
-          <t>789c3558c73ed5654b562b424681009a</t>
+          <t>5301bbc32276ce7d3caf98531cc72308</t>
         </is>
       </c>
       <c r="B511" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Merluccius bilinearis</t>
         </is>
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Silver hake</t>
         </is>
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E511">
@@ -14672,17 +14672,17 @@
     <row r="512">
       <c r="A512" t="inlineStr">
         <is>
-          <t>d3cde07a54f7a06587624ecccc269000</t>
+          <t>d1037cb2974d16fd6737caf7d268aea3</t>
         </is>
       </c>
       <c r="B512" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Peprilus triacanthus</t>
         </is>
       </c>
       <c r="C512" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>American butterfish</t>
         </is>
       </c>
       <c r="D512" t="inlineStr">
@@ -14700,17 +14700,17 @@
     <row r="513">
       <c r="A513" t="inlineStr">
         <is>
-          <t>d1037cb2974d16fd6737caf7d268aea3</t>
+          <t>d3cde07a54f7a06587624ecccc269000</t>
         </is>
       </c>
       <c r="B513" t="inlineStr">
         <is>
-          <t>Peprilus triacanthus</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C513" t="inlineStr">
         <is>
-          <t>American butterfish</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D513" t="inlineStr">
@@ -15120,17 +15120,17 @@
     <row r="528">
       <c r="A528" t="inlineStr">
         <is>
-          <t>839ce4fd327b30b019c9bcdd6e1b2de5</t>
+          <t>2e9e2e962df3f0038df2fe0312c479dc</t>
         </is>
       </c>
       <c r="B528" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Morone saxatilis</t>
         </is>
       </c>
       <c r="C528" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Striped bass</t>
         </is>
       </c>
       <c r="D528" t="inlineStr">
@@ -15148,17 +15148,17 @@
     <row r="529">
       <c r="A529" t="inlineStr">
         <is>
-          <t>2e9e2e962df3f0038df2fe0312c479dc</t>
+          <t>839ce4fd327b30b019c9bcdd6e1b2de5</t>
         </is>
       </c>
       <c r="B529" t="inlineStr">
         <is>
-          <t>Morone saxatilis</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C529" t="inlineStr">
         <is>
-          <t>Striped bass</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D529" t="inlineStr">
@@ -15372,17 +15372,17 @@
     <row r="537">
       <c r="A537" t="inlineStr">
         <is>
-          <t>7ce3896add3d274d8fc1c4aa40859b8c</t>
+          <t>418749d4b591b1b25dac38bf31e3d9fd</t>
         </is>
       </c>
       <c r="B537" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C537" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D537" t="inlineStr">
@@ -15400,17 +15400,17 @@
     <row r="538">
       <c r="A538" t="inlineStr">
         <is>
-          <t>418749d4b591b1b25dac38bf31e3d9fd</t>
+          <t>7ce3896add3d274d8fc1c4aa40859b8c</t>
         </is>
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C538" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D538" t="inlineStr">
@@ -15456,17 +15456,17 @@
     <row r="540">
       <c r="A540" t="inlineStr">
         <is>
-          <t>02b6299a10281a10b918164ab3318ccf</t>
+          <t>335c0344d065a4fec25599bff157fa5e</t>
         </is>
       </c>
       <c r="B540" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C540" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D540" t="inlineStr">
@@ -15484,17 +15484,17 @@
     <row r="541">
       <c r="A541" t="inlineStr">
         <is>
-          <t>335c0344d065a4fec25599bff157fa5e</t>
+          <t>02b6299a10281a10b918164ab3318ccf</t>
         </is>
       </c>
       <c r="B541" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C541" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D541" t="inlineStr">
@@ -15634,7 +15634,7 @@
       </c>
       <c r="C546" t="inlineStr">
         <is>
-          <t>Pig</t>
+          <t>Wild boar</t>
         </is>
       </c>
       <c r="D546" t="inlineStr">
@@ -16044,17 +16044,17 @@
     <row r="561">
       <c r="A561" t="inlineStr">
         <is>
-          <t>cdb99595d4754adaf7ada4436ef01afb</t>
+          <t>e22e31015487c6672136e0a34500ba74</t>
         </is>
       </c>
       <c r="B561" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C561" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D561" t="inlineStr">
@@ -16072,17 +16072,17 @@
     <row r="562">
       <c r="A562" t="inlineStr">
         <is>
-          <t>e22e31015487c6672136e0a34500ba74</t>
+          <t>cdb99595d4754adaf7ada4436ef01afb</t>
         </is>
       </c>
       <c r="B562" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C562" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D562" t="inlineStr">
@@ -16100,17 +16100,17 @@
     <row r="563">
       <c r="A563" t="inlineStr">
         <is>
-          <t>9a2a72396f99efc65bc69b963600375e</t>
+          <t>c18de91ef963edb02cb38cd4ddd35dcd</t>
         </is>
       </c>
       <c r="B563" t="inlineStr">
         <is>
-          <t>Ammodytes americanus or hexapterus</t>
+          <t>Anguilla rostrata</t>
         </is>
       </c>
       <c r="C563" t="inlineStr">
         <is>
-          <t>American or Pacific sand lance</t>
+          <t>American eel</t>
         </is>
       </c>
       <c r="D563" t="inlineStr">
@@ -16128,17 +16128,17 @@
     <row r="564">
       <c r="A564" t="inlineStr">
         <is>
-          <t>c18de91ef963edb02cb38cd4ddd35dcd</t>
+          <t>9a2a72396f99efc65bc69b963600375e</t>
         </is>
       </c>
       <c r="B564" t="inlineStr">
         <is>
-          <t>Anguilla rostrata</t>
+          <t>Ammodytes americanus or hexapterus</t>
         </is>
       </c>
       <c r="C564" t="inlineStr">
         <is>
-          <t>American eel</t>
+          <t>American or Pacific sand lance</t>
         </is>
       </c>
       <c r="D564" t="inlineStr">
@@ -16240,17 +16240,17 @@
     <row r="568">
       <c r="A568" t="inlineStr">
         <is>
-          <t>894d651908b33097ed7c5df271903daa</t>
+          <t>5432a6e652c21bb79c110c1179832080</t>
         </is>
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D568" t="inlineStr">
@@ -16268,17 +16268,17 @@
     <row r="569">
       <c r="A569" t="inlineStr">
         <is>
-          <t>5432a6e652c21bb79c110c1179832080</t>
+          <t>894d651908b33097ed7c5df271903daa</t>
         </is>
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D569" t="inlineStr">
@@ -16660,17 +16660,17 @@
     <row r="583">
       <c r="A583" t="inlineStr">
         <is>
-          <t>46db97c5565c94eb6c74f3e91483addd</t>
+          <t>13aaa8dbc5a17d7bcb3decd110443daa</t>
         </is>
       </c>
       <c r="B583" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C583" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D583" t="inlineStr">
@@ -16688,17 +16688,17 @@
     <row r="584">
       <c r="A584" t="inlineStr">
         <is>
-          <t>13aaa8dbc5a17d7bcb3decd110443daa</t>
+          <t>46db97c5565c94eb6c74f3e91483addd</t>
         </is>
       </c>
       <c r="B584" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C584" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D584" t="inlineStr">
@@ -16968,17 +16968,17 @@
     <row r="594">
       <c r="A594" t="inlineStr">
         <is>
-          <t>6c7006c06aa32fc683ae452c58d0bebb</t>
+          <t>ffd849bcb52bcd32cbb308ffe3a5ab64</t>
         </is>
       </c>
       <c r="B594" t="inlineStr">
         <is>
-          <t>Syngnathus fuscus</t>
+          <t>Prionotus carolinus</t>
         </is>
       </c>
       <c r="C594" t="inlineStr">
         <is>
-          <t>Northern pipefish</t>
+          <t>Northern sea robin</t>
         </is>
       </c>
       <c r="D594" t="inlineStr">
@@ -16996,17 +16996,17 @@
     <row r="595">
       <c r="A595" t="inlineStr">
         <is>
-          <t>ffd849bcb52bcd32cbb308ffe3a5ab64</t>
+          <t>6c7006c06aa32fc683ae452c58d0bebb</t>
         </is>
       </c>
       <c r="B595" t="inlineStr">
         <is>
-          <t>Prionotus carolinus</t>
+          <t>Syngnathus fuscus</t>
         </is>
       </c>
       <c r="C595" t="inlineStr">
         <is>
-          <t>Northern sea robin</t>
+          <t>Northern pipefish</t>
         </is>
       </c>
       <c r="D595" t="inlineStr">
@@ -17192,17 +17192,17 @@
     <row r="602">
       <c r="A602" t="inlineStr">
         <is>
-          <t>767468fa4beea0afb40e5256c49c0b93</t>
+          <t>8611083ec600c411702bc68a9153104e</t>
         </is>
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>Merluccius bilinearis</t>
+          <t>Anguilla rostrata</t>
         </is>
       </c>
       <c r="C602" t="inlineStr">
         <is>
-          <t>Silver hake</t>
+          <t>American eel</t>
         </is>
       </c>
       <c r="D602" t="inlineStr">
@@ -17220,22 +17220,22 @@
     <row r="603">
       <c r="A603" t="inlineStr">
         <is>
-          <t>8611083ec600c411702bc68a9153104e</t>
+          <t>9b17bc093b1306fd3505f3d397cf5e73</t>
         </is>
       </c>
       <c r="B603" t="inlineStr">
         <is>
-          <t>Anguilla rostrata</t>
+          <t>Gallus gallus</t>
         </is>
       </c>
       <c r="C603" t="inlineStr">
         <is>
-          <t>American eel</t>
+          <t>Chicken</t>
         </is>
       </c>
       <c r="D603" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E603">
@@ -17248,22 +17248,22 @@
     <row r="604">
       <c r="A604" t="inlineStr">
         <is>
-          <t>2cae1e97dfea33fd1317d7c693cab07d</t>
+          <t>767468fa4beea0afb40e5256c49c0b93</t>
         </is>
       </c>
       <c r="B604" t="inlineStr">
         <is>
-          <t>Anas sp</t>
+          <t>Merluccius bilinearis</t>
         </is>
       </c>
       <c r="C604" t="inlineStr">
         <is>
-          <t>Mallard sp</t>
+          <t>Silver hake</t>
         </is>
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E604">
@@ -17276,22 +17276,22 @@
     <row r="605">
       <c r="A605" t="inlineStr">
         <is>
-          <t>9b17bc093b1306fd3505f3d397cf5e73</t>
+          <t>2cae1e97dfea33fd1317d7c693cab07d</t>
         </is>
       </c>
       <c r="B605" t="inlineStr">
         <is>
-          <t>Gallus gallus</t>
+          <t>Anas sp</t>
         </is>
       </c>
       <c r="C605" t="inlineStr">
         <is>
-          <t>Chicken</t>
+          <t>Mallard sp</t>
         </is>
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E605">
@@ -17528,22 +17528,22 @@
     <row r="614">
       <c r="A614" t="inlineStr">
         <is>
-          <t>e20ba3459c89adb98e25cfe29d83b420</t>
+          <t>81f442b9b2664646a2966f2cb41bfbc6</t>
         </is>
       </c>
       <c r="B614" t="inlineStr">
         <is>
-          <t>Cetorhinus maximus</t>
+          <t>Paralichthys dentatus</t>
         </is>
       </c>
       <c r="C614" t="inlineStr">
         <is>
-          <t>Basking shark</t>
+          <t>Summer flounder</t>
         </is>
       </c>
       <c r="D614" t="inlineStr">
         <is>
-          <t>Elasmobranch</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E614">
@@ -17556,22 +17556,22 @@
     <row r="615">
       <c r="A615" t="inlineStr">
         <is>
-          <t>81f442b9b2664646a2966f2cb41bfbc6</t>
+          <t>e20ba3459c89adb98e25cfe29d83b420</t>
         </is>
       </c>
       <c r="B615" t="inlineStr">
         <is>
-          <t>Paralichthys dentatus</t>
+          <t>Cetorhinus maximus</t>
         </is>
       </c>
       <c r="C615" t="inlineStr">
         <is>
-          <t>Summer flounder</t>
+          <t>Basking shark</t>
         </is>
       </c>
       <c r="D615" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Elasmobranch</t>
         </is>
       </c>
       <c r="E615">
@@ -18088,22 +18088,22 @@
     <row r="634">
       <c r="A634" t="inlineStr">
         <is>
-          <t>22f00d0359bb77921d5b2a33334af24e</t>
+          <t>dab44add09b99f92b3bfc5ec53848737</t>
         </is>
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Peprilus triacanthus</t>
         </is>
       </c>
       <c r="C634" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>American butterfish</t>
         </is>
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E634">
@@ -18116,22 +18116,22 @@
     <row r="635">
       <c r="A635" t="inlineStr">
         <is>
-          <t>dab44add09b99f92b3bfc5ec53848737</t>
+          <t>22f00d0359bb77921d5b2a33334af24e</t>
         </is>
       </c>
       <c r="B635" t="inlineStr">
         <is>
-          <t>Peprilus triacanthus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C635" t="inlineStr">
         <is>
-          <t>American butterfish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E635">
@@ -18284,17 +18284,17 @@
     <row r="641">
       <c r="A641" t="inlineStr">
         <is>
-          <t>d1c7b1476c27001b8d256eb958915991</t>
+          <t>63c9de6f692725be4edd26028f883e0a</t>
         </is>
       </c>
       <c r="B641" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C641" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D641" t="inlineStr">
@@ -18312,17 +18312,17 @@
     <row r="642">
       <c r="A642" t="inlineStr">
         <is>
-          <t>63c9de6f692725be4edd26028f883e0a</t>
+          <t>d1c7b1476c27001b8d256eb958915991</t>
         </is>
       </c>
       <c r="B642" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C642" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D642" t="inlineStr">
@@ -18452,17 +18452,17 @@
     <row r="647">
       <c r="A647" t="inlineStr">
         <is>
-          <t>5345f67eb49c7d23457a7a2189bd8d07</t>
+          <t>0c1939639b84375649f7bb8b9ee8ae2d</t>
         </is>
       </c>
       <c r="B647" t="inlineStr">
         <is>
-          <t>Felis catus</t>
+          <t>Sus scrofa</t>
         </is>
       </c>
       <c r="C647" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Wild boar</t>
         </is>
       </c>
       <c r="D647" t="inlineStr">
@@ -18480,17 +18480,17 @@
     <row r="648">
       <c r="A648" t="inlineStr">
         <is>
-          <t>0c1939639b84375649f7bb8b9ee8ae2d</t>
+          <t>5345f67eb49c7d23457a7a2189bd8d07</t>
         </is>
       </c>
       <c r="B648" t="inlineStr">
         <is>
-          <t>Sus scrofa</t>
+          <t>Felis catus</t>
         </is>
       </c>
       <c r="C648" t="inlineStr">
         <is>
-          <t>Pig</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D648" t="inlineStr">
@@ -18816,17 +18816,17 @@
     <row r="660">
       <c r="A660" t="inlineStr">
         <is>
-          <t>118de0da9053ad27ad0e3c1e136454d9</t>
+          <t>852758a2afb6b5be4e13423448357d97</t>
         </is>
       </c>
       <c r="B660" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Tautoga onitis</t>
         </is>
       </c>
       <c r="C660" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Tautog</t>
         </is>
       </c>
       <c r="D660" t="inlineStr">
@@ -18844,17 +18844,17 @@
     <row r="661">
       <c r="A661" t="inlineStr">
         <is>
-          <t>852758a2afb6b5be4e13423448357d97</t>
+          <t>118de0da9053ad27ad0e3c1e136454d9</t>
         </is>
       </c>
       <c r="B661" t="inlineStr">
         <is>
-          <t>Tautoga onitis</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C661" t="inlineStr">
         <is>
-          <t>Tautog</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D661" t="inlineStr">
@@ -19096,17 +19096,17 @@
     <row r="670">
       <c r="A670" t="inlineStr">
         <is>
-          <t>91f820c7f5a5f2adfce817262dcc8bfe</t>
+          <t>565faaf311255e6253e5941fc7cbde17</t>
         </is>
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D670" t="inlineStr">
@@ -19124,17 +19124,17 @@
     <row r="671">
       <c r="A671" t="inlineStr">
         <is>
-          <t>565faaf311255e6253e5941fc7cbde17</t>
+          <t>91f820c7f5a5f2adfce817262dcc8bfe</t>
         </is>
       </c>
       <c r="B671" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C671" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D671" t="inlineStr">
@@ -19236,22 +19236,22 @@
     <row r="675">
       <c r="A675" t="inlineStr">
         <is>
-          <t>a4a495dca8d3677dc8e9fb34a25824f2</t>
+          <t>a96ef4edd749d4ad72ea06edc9f46fbd</t>
         </is>
       </c>
       <c r="B675" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C675" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D675" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E675">
@@ -19264,22 +19264,22 @@
     <row r="676">
       <c r="A676" t="inlineStr">
         <is>
-          <t>a96ef4edd749d4ad72ea06edc9f46fbd</t>
+          <t>a4a495dca8d3677dc8e9fb34a25824f2</t>
         </is>
       </c>
       <c r="B676" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C676" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D676" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E676">
@@ -19404,22 +19404,22 @@
     <row r="681">
       <c r="A681" t="inlineStr">
         <is>
-          <t>b996740838ef8198336ac30138ca5108</t>
+          <t>d81ad13bba54c523bb1787e45dfb9651</t>
         </is>
       </c>
       <c r="B681" t="inlineStr">
         <is>
-          <t>Tautoga onitis</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C681" t="inlineStr">
         <is>
-          <t>Tautog</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D681" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E681">
@@ -19432,22 +19432,22 @@
     <row r="682">
       <c r="A682" t="inlineStr">
         <is>
-          <t>3ab4134a0a8cde924b9aa3b1f8ea99b0</t>
+          <t>b996740838ef8198336ac30138ca5108</t>
         </is>
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>Aythya sp</t>
+          <t>Tautoga onitis</t>
         </is>
       </c>
       <c r="C682" t="inlineStr">
         <is>
-          <t>Duck sp</t>
+          <t>Tautog</t>
         </is>
       </c>
       <c r="D682" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E682">
@@ -19460,22 +19460,22 @@
     <row r="683">
       <c r="A683" t="inlineStr">
         <is>
-          <t>d81ad13bba54c523bb1787e45dfb9651</t>
+          <t>3ab4134a0a8cde924b9aa3b1f8ea99b0</t>
         </is>
       </c>
       <c r="B683" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Aythya sp</t>
         </is>
       </c>
       <c r="C683" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Duck sp</t>
         </is>
       </c>
       <c r="D683" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E683">
@@ -19610,7 +19610,7 @@
       </c>
       <c r="C688" t="inlineStr">
         <is>
-          <t>Pig</t>
+          <t>Wild boar</t>
         </is>
       </c>
       <c r="D688" t="inlineStr">
@@ -19992,7 +19992,7 @@
     <row r="702">
       <c r="A702" t="inlineStr">
         <is>
-          <t>942122125dfa6046a9eb826c40b9d6da</t>
+          <t>22a5133369dccbe25ef8c3bda50ad263</t>
         </is>
       </c>
       <c r="B702" t="inlineStr">
@@ -20020,17 +20020,17 @@
     <row r="703">
       <c r="A703" t="inlineStr">
         <is>
-          <t>22a5133369dccbe25ef8c3bda50ad263</t>
+          <t>1c6f0b91a9d79b241a6dbc424e8f50c4</t>
         </is>
       </c>
       <c r="B703" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Morone saxatilis</t>
         </is>
       </c>
       <c r="C703" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Striped bass</t>
         </is>
       </c>
       <c r="D703" t="inlineStr">
@@ -20048,17 +20048,17 @@
     <row r="704">
       <c r="A704" t="inlineStr">
         <is>
-          <t>1c6f0b91a9d79b241a6dbc424e8f50c4</t>
+          <t>942122125dfa6046a9eb826c40b9d6da</t>
         </is>
       </c>
       <c r="B704" t="inlineStr">
         <is>
-          <t>Morone saxatilis</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C704" t="inlineStr">
         <is>
-          <t>Striped bass</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D704" t="inlineStr">
@@ -20244,22 +20244,22 @@
     <row r="711">
       <c r="A711" t="inlineStr">
         <is>
-          <t>2b1707c23de2672a2cef049f6443aaf6</t>
+          <t>6eb04fb0bc1cc0fd1fb13c3192f24223</t>
         </is>
       </c>
       <c r="B711" t="inlineStr">
         <is>
-          <t>Anatidae sp</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C711" t="inlineStr">
         <is>
-          <t>Duck geese or swan</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D711" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E711">
@@ -20272,22 +20272,22 @@
     <row r="712">
       <c r="A712" t="inlineStr">
         <is>
-          <t>6eb04fb0bc1cc0fd1fb13c3192f24223</t>
+          <t>2b1707c23de2672a2cef049f6443aaf6</t>
         </is>
       </c>
       <c r="B712" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Anatidae sp</t>
         </is>
       </c>
       <c r="C712" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Duck geese or swan</t>
         </is>
       </c>
       <c r="D712" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E712">
@@ -20468,17 +20468,17 @@
     <row r="719">
       <c r="A719" t="inlineStr">
         <is>
-          <t>0c8fbc8c386a06204703c0b9d12dbd71</t>
+          <t>6a83eb23e34e01773abb7d038e38c583</t>
         </is>
       </c>
       <c r="B719" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C719" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D719" t="inlineStr">
@@ -20496,17 +20496,17 @@
     <row r="720">
       <c r="A720" t="inlineStr">
         <is>
-          <t>6a83eb23e34e01773abb7d038e38c583</t>
+          <t>0c8fbc8c386a06204703c0b9d12dbd71</t>
         </is>
       </c>
       <c r="B720" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C720" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D720" t="inlineStr">
@@ -20720,7 +20720,7 @@
     <row r="728">
       <c r="A728" t="inlineStr">
         <is>
-          <t>fc5fd999093ec0245ae3fb9ad8bfa92d</t>
+          <t>2dc9ab01e95dfd0e49b7e14454a96178</t>
         </is>
       </c>
       <c r="B728" t="inlineStr">
@@ -20748,7 +20748,7 @@
     <row r="729">
       <c r="A729" t="inlineStr">
         <is>
-          <t>2dc9ab01e95dfd0e49b7e14454a96178</t>
+          <t>fc5fd999093ec0245ae3fb9ad8bfa92d</t>
         </is>
       </c>
       <c r="B729" t="inlineStr">
@@ -20888,22 +20888,22 @@
     <row r="734">
       <c r="A734" t="inlineStr">
         <is>
-          <t>8e4e4ceebdf28e1f7160a3a555a4ef1b</t>
+          <t>879e754a58aca523d2a744a9e14edf50</t>
         </is>
       </c>
       <c r="B734" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Peprilus triacanthus</t>
         </is>
       </c>
       <c r="C734" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>American butterfish</t>
         </is>
       </c>
       <c r="D734" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E734">
@@ -20916,22 +20916,22 @@
     <row r="735">
       <c r="A735" t="inlineStr">
         <is>
-          <t>879e754a58aca523d2a744a9e14edf50</t>
+          <t>8e4e4ceebdf28e1f7160a3a555a4ef1b</t>
         </is>
       </c>
       <c r="B735" t="inlineStr">
         <is>
-          <t>Peprilus triacanthus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C735" t="inlineStr">
         <is>
-          <t>American butterfish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D735" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E735">
@@ -21084,22 +21084,22 @@
     <row r="741">
       <c r="A741" t="inlineStr">
         <is>
-          <t>eaa5768bab15d36998bee97a0de43ad3</t>
+          <t>2608f30bab2abeaa588c31304e988dc1</t>
         </is>
       </c>
       <c r="B741" t="inlineStr">
         <is>
-          <t>Felis catus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C741" t="inlineStr">
         <is>
-          <t>Cat</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D741" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E741">
@@ -21140,22 +21140,22 @@
     <row r="743">
       <c r="A743" t="inlineStr">
         <is>
-          <t>2608f30bab2abeaa588c31304e988dc1</t>
+          <t>eaa5768bab15d36998bee97a0de43ad3</t>
         </is>
       </c>
       <c r="B743" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Felis catus</t>
         </is>
       </c>
       <c r="C743" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Cat</t>
         </is>
       </c>
       <c r="D743" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E743">
@@ -21168,22 +21168,22 @@
     <row r="744">
       <c r="A744" t="inlineStr">
         <is>
-          <t>413af729da58aef621f28aa666578aac</t>
+          <t>e5d62629742b301c8b25ac58f4392651</t>
         </is>
       </c>
       <c r="B744" t="inlineStr">
         <is>
-          <t>Scophthalmus aquosus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C744" t="inlineStr">
         <is>
-          <t>Windowpane flounder</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D744" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E744">
@@ -21196,22 +21196,22 @@
     <row r="745">
       <c r="A745" t="inlineStr">
         <is>
-          <t>e5d62629742b301c8b25ac58f4392651</t>
+          <t>413af729da58aef621f28aa666578aac</t>
         </is>
       </c>
       <c r="B745" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Scophthalmus aquosus</t>
         </is>
       </c>
       <c r="C745" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Windowpane flounder</t>
         </is>
       </c>
       <c r="D745" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E745">
@@ -21252,17 +21252,17 @@
     <row r="747">
       <c r="A747" t="inlineStr">
         <is>
-          <t>5b2278535af7a77c15966bc43d0188bd</t>
+          <t>3acbe8e8eeda501fa38d27f4aae7b1c8</t>
         </is>
       </c>
       <c r="B747" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C747" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D747" t="inlineStr">
@@ -21280,17 +21280,17 @@
     <row r="748">
       <c r="A748" t="inlineStr">
         <is>
-          <t>3acbe8e8eeda501fa38d27f4aae7b1c8</t>
+          <t>5b2278535af7a77c15966bc43d0188bd</t>
         </is>
       </c>
       <c r="B748" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C748" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D748" t="inlineStr">
@@ -21308,22 +21308,22 @@
     <row r="749">
       <c r="A749" t="inlineStr">
         <is>
-          <t>f79aca241011d34a53151a12d9fb4fd1</t>
+          <t>8d4c237bc0ebd7322d1c46c825c7843b</t>
         </is>
       </c>
       <c r="B749" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Anatidae sp</t>
         </is>
       </c>
       <c r="C749" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Duck geese or swan</t>
         </is>
       </c>
       <c r="D749" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E749">
@@ -21336,22 +21336,22 @@
     <row r="750">
       <c r="A750" t="inlineStr">
         <is>
-          <t>8d4c237bc0ebd7322d1c46c825c7843b</t>
+          <t>f79aca241011d34a53151a12d9fb4fd1</t>
         </is>
       </c>
       <c r="B750" t="inlineStr">
         <is>
-          <t>Anatidae sp</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C750" t="inlineStr">
         <is>
-          <t>Duck geese or swan</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D750" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E750">
@@ -21560,7 +21560,7 @@
     <row r="758">
       <c r="A758" t="inlineStr">
         <is>
-          <t>2b663b17ee54d1b2b9cb4ef45176be13</t>
+          <t>832d50e383e748f9f6c2c19624236208</t>
         </is>
       </c>
       <c r="B758" t="inlineStr">
@@ -21588,7 +21588,7 @@
     <row r="759">
       <c r="A759" t="inlineStr">
         <is>
-          <t>832d50e383e748f9f6c2c19624236208</t>
+          <t>2b663b17ee54d1b2b9cb4ef45176be13</t>
         </is>
       </c>
       <c r="B759" t="inlineStr">
@@ -22148,22 +22148,22 @@
     <row r="779">
       <c r="A779" t="inlineStr">
         <is>
-          <t>2ee81e646ca3572397051907472a9313</t>
+          <t>eadee0f7aca47c5a749b23a824369709</t>
         </is>
       </c>
       <c r="B779" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C779" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D779" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E779">
@@ -22176,22 +22176,22 @@
     <row r="780">
       <c r="A780" t="inlineStr">
         <is>
-          <t>eadee0f7aca47c5a749b23a824369709</t>
+          <t>2ee81e646ca3572397051907472a9313</t>
         </is>
       </c>
       <c r="B780" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C780" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D780" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E780">
@@ -22400,17 +22400,17 @@
     <row r="788">
       <c r="A788" t="inlineStr">
         <is>
-          <t>88de9a17f027cc5e53358f9739a0e7a1</t>
+          <t>079fb139d03e392c1028efa267e54d00</t>
         </is>
       </c>
       <c r="B788" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Merluccius bilinearis</t>
         </is>
       </c>
       <c r="C788" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Silver hake</t>
         </is>
       </c>
       <c r="D788" t="inlineStr">
@@ -22428,17 +22428,17 @@
     <row r="789">
       <c r="A789" t="inlineStr">
         <is>
-          <t>079fb139d03e392c1028efa267e54d00</t>
+          <t>88de9a17f027cc5e53358f9739a0e7a1</t>
         </is>
       </c>
       <c r="B789" t="inlineStr">
         <is>
-          <t>Merluccius bilinearis</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C789" t="inlineStr">
         <is>
-          <t>Silver hake</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D789" t="inlineStr">
@@ -22512,17 +22512,17 @@
     <row r="792">
       <c r="A792" t="inlineStr">
         <is>
-          <t>7c4e10f6103988e705c8c5765d9fdaa3</t>
+          <t>edb9d268bcd8c98c86bd7e8971544fe1</t>
         </is>
       </c>
       <c r="B792" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C792" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D792" t="inlineStr">
@@ -22540,17 +22540,17 @@
     <row r="793">
       <c r="A793" t="inlineStr">
         <is>
-          <t>edb9d268bcd8c98c86bd7e8971544fe1</t>
+          <t>7c4e10f6103988e705c8c5765d9fdaa3</t>
         </is>
       </c>
       <c r="B793" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C793" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D793" t="inlineStr">
@@ -22624,17 +22624,17 @@
     <row r="796">
       <c r="A796" t="inlineStr">
         <is>
-          <t>e7863beee89b31bb10173713c704684c</t>
+          <t>503e037b41c0c13e76928b9d2fe24c23</t>
         </is>
       </c>
       <c r="B796" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C796" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D796" t="inlineStr">
@@ -22680,17 +22680,17 @@
     <row r="798">
       <c r="A798" t="inlineStr">
         <is>
-          <t>503e037b41c0c13e76928b9d2fe24c23</t>
+          <t>e7863beee89b31bb10173713c704684c</t>
         </is>
       </c>
       <c r="B798" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D798" t="inlineStr">
@@ -22820,22 +22820,22 @@
     <row r="803">
       <c r="A803" t="inlineStr">
         <is>
-          <t>267d361028b5d98f0610470de52f3135</t>
+          <t>3aaa4a4f171b0c6da1d76f1c85bd6ae9</t>
         </is>
       </c>
       <c r="B803" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Peprilus triacanthus</t>
         </is>
       </c>
       <c r="C803" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>American butterfish</t>
         </is>
       </c>
       <c r="D803" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E803">
@@ -22848,22 +22848,22 @@
     <row r="804">
       <c r="A804" t="inlineStr">
         <is>
-          <t>3aaa4a4f171b0c6da1d76f1c85bd6ae9</t>
+          <t>267d361028b5d98f0610470de52f3135</t>
         </is>
       </c>
       <c r="B804" t="inlineStr">
         <is>
-          <t>Peprilus triacanthus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C804" t="inlineStr">
         <is>
-          <t>American butterfish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D804" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E804">
@@ -23044,17 +23044,17 @@
     <row r="811">
       <c r="A811" t="inlineStr">
         <is>
-          <t>feac75b1d61a3b01472bf2397bcb1053</t>
+          <t>543ae87e917382be78718dfb365f8e20</t>
         </is>
       </c>
       <c r="B811" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C811" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D811" t="inlineStr">
@@ -23072,17 +23072,17 @@
     <row r="812">
       <c r="A812" t="inlineStr">
         <is>
-          <t>543ae87e917382be78718dfb365f8e20</t>
+          <t>feac75b1d61a3b01472bf2397bcb1053</t>
         </is>
       </c>
       <c r="B812" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C812" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D812" t="inlineStr">
@@ -23212,22 +23212,22 @@
     <row r="817">
       <c r="A817" t="inlineStr">
         <is>
-          <t>20cbad0c5110637dac101a5a6afb76a3</t>
+          <t>64a4b34bcf5026fb61a08b66e32f601d</t>
         </is>
       </c>
       <c r="B817" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C817" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D817" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E817">
@@ -23240,22 +23240,22 @@
     <row r="818">
       <c r="A818" t="inlineStr">
         <is>
-          <t>64a4b34bcf5026fb61a08b66e32f601d</t>
+          <t>20cbad0c5110637dac101a5a6afb76a3</t>
         </is>
       </c>
       <c r="B818" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C818" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D818" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E818">
@@ -23268,17 +23268,17 @@
     <row r="819">
       <c r="A819" t="inlineStr">
         <is>
-          <t>338462173b822c7e2b9bafa8a9c0f4d3</t>
+          <t>f836ca1f26a5422d74765bb4513b6d0b</t>
         </is>
       </c>
       <c r="B819" t="inlineStr">
         <is>
-          <t>Tautogolabrus adspersus</t>
+          <t>Prionotus carolinus</t>
         </is>
       </c>
       <c r="C819" t="inlineStr">
         <is>
-          <t>Cunner</t>
+          <t>Northern sea robin</t>
         </is>
       </c>
       <c r="D819" t="inlineStr">
@@ -23296,17 +23296,17 @@
     <row r="820">
       <c r="A820" t="inlineStr">
         <is>
-          <t>7ee102ea6b4263ac841924fc5250217f</t>
+          <t>338462173b822c7e2b9bafa8a9c0f4d3</t>
         </is>
       </c>
       <c r="B820" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Tautogolabrus adspersus</t>
         </is>
       </c>
       <c r="C820" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Cunner</t>
         </is>
       </c>
       <c r="D820" t="inlineStr">
@@ -23324,17 +23324,17 @@
     <row r="821">
       <c r="A821" t="inlineStr">
         <is>
-          <t>f836ca1f26a5422d74765bb4513b6d0b</t>
+          <t>7ee102ea6b4263ac841924fc5250217f</t>
         </is>
       </c>
       <c r="B821" t="inlineStr">
         <is>
-          <t>Prionotus carolinus</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C821" t="inlineStr">
         <is>
-          <t>Northern sea robin</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D821" t="inlineStr">
@@ -23380,22 +23380,22 @@
     <row r="823">
       <c r="A823" t="inlineStr">
         <is>
-          <t>4c14a46603e606b723c16c23351ab9dd</t>
+          <t>ab97a9a9559c88558c38aa6b723d8f8b</t>
         </is>
       </c>
       <c r="B823" t="inlineStr">
         <is>
-          <t>Zenopsis conchifera</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C823" t="inlineStr">
         <is>
-          <t>Buckler dory</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D823" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E823">
@@ -23408,22 +23408,22 @@
     <row r="824">
       <c r="A824" t="inlineStr">
         <is>
-          <t>ab97a9a9559c88558c38aa6b723d8f8b</t>
+          <t>4c14a46603e606b723c16c23351ab9dd</t>
         </is>
       </c>
       <c r="B824" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Zenopsis conchifera</t>
         </is>
       </c>
       <c r="C824" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Buckler dory</t>
         </is>
       </c>
       <c r="D824" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E824">
@@ -23548,22 +23548,22 @@
     <row r="829">
       <c r="A829" t="inlineStr">
         <is>
-          <t>636ef55278f639540cf3380bbb5c9212</t>
+          <t>bc6c70c1cdde3054da49619121d9d53b</t>
         </is>
       </c>
       <c r="B829" t="inlineStr">
         <is>
-          <t>Delphinus delphis</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C829" t="inlineStr">
         <is>
-          <t>Shortbeaked common dolphin</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D829" t="inlineStr">
         <is>
-          <t>Marine Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E829">
@@ -23576,22 +23576,22 @@
     <row r="830">
       <c r="A830" t="inlineStr">
         <is>
-          <t>bc6c70c1cdde3054da49619121d9d53b</t>
+          <t>636ef55278f639540cf3380bbb5c9212</t>
         </is>
       </c>
       <c r="B830" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Delphinus delphis</t>
         </is>
       </c>
       <c r="C830" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Shortbeaked common dolphin</t>
         </is>
       </c>
       <c r="D830" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Marine Mammal</t>
         </is>
       </c>
       <c r="E830">
@@ -23688,22 +23688,22 @@
     <row r="834">
       <c r="A834" t="inlineStr">
         <is>
-          <t>820d3e0051268c4f73f8f13e1de1dd42</t>
+          <t>f507349f89870cbfa22cf775c9ac809d</t>
         </is>
       </c>
       <c r="B834" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C834" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D834" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E834">
@@ -23716,22 +23716,22 @@
     <row r="835">
       <c r="A835" t="inlineStr">
         <is>
-          <t>f507349f89870cbfa22cf775c9ac809d</t>
+          <t>7a14c891c696cf299f93eb09be0b4141</t>
         </is>
       </c>
       <c r="B835" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C835" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D835" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E835">
@@ -23744,7 +23744,7 @@
     <row r="836">
       <c r="A836" t="inlineStr">
         <is>
-          <t>7a14c891c696cf299f93eb09be0b4141</t>
+          <t>820d3e0051268c4f73f8f13e1de1dd42</t>
         </is>
       </c>
       <c r="B836" t="inlineStr">
@@ -23772,17 +23772,17 @@
     <row r="837">
       <c r="A837" t="inlineStr">
         <is>
-          <t>7c09c4738bb5520ae2da1102a2b10718</t>
+          <t>61586204df80e009b4fb5bfe1ceda644</t>
         </is>
       </c>
       <c r="B837" t="inlineStr">
         <is>
-          <t>Cottidae sp</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C837" t="inlineStr">
         <is>
-          <t>Sculpins</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D837" t="inlineStr">
@@ -23800,17 +23800,17 @@
     <row r="838">
       <c r="A838" t="inlineStr">
         <is>
-          <t>61586204df80e009b4fb5bfe1ceda644</t>
+          <t>7c09c4738bb5520ae2da1102a2b10718</t>
         </is>
       </c>
       <c r="B838" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Cottidae sp</t>
         </is>
       </c>
       <c r="C838" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Sculpins</t>
         </is>
       </c>
       <c r="D838" t="inlineStr">
@@ -24416,22 +24416,22 @@
     <row r="860">
       <c r="A860" t="inlineStr">
         <is>
-          <t>8b9988a796bd30179970d9349e5c9299</t>
+          <t>46c40f0ff72fabb6f49280e33c7af225</t>
         </is>
       </c>
       <c r="B860" t="inlineStr">
         <is>
-          <t>Bos taurus</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C860" t="inlineStr">
         <is>
-          <t>Cow</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D860" t="inlineStr">
         <is>
-          <t>Livestock</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E860">
@@ -24444,17 +24444,17 @@
     <row r="861">
       <c r="A861" t="inlineStr">
         <is>
-          <t>46c40f0ff72fabb6f49280e33c7af225</t>
+          <t>9d282340656706c6622517bc67a2e903</t>
         </is>
       </c>
       <c r="B861" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Fundulus heteroclitus or majalis</t>
         </is>
       </c>
       <c r="C861" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Mummichog or striped killifish</t>
         </is>
       </c>
       <c r="D861" t="inlineStr">
@@ -24472,22 +24472,22 @@
     <row r="862">
       <c r="A862" t="inlineStr">
         <is>
-          <t>9d282340656706c6622517bc67a2e903</t>
+          <t>8b9988a796bd30179970d9349e5c9299</t>
         </is>
       </c>
       <c r="B862" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus or majalis</t>
+          <t>Bos taurus</t>
         </is>
       </c>
       <c r="C862" t="inlineStr">
         <is>
-          <t>Mummichog or striped killifish</t>
+          <t>Cow</t>
         </is>
       </c>
       <c r="D862" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Livestock</t>
         </is>
       </c>
       <c r="E862">
@@ -24584,17 +24584,17 @@
     <row r="866">
       <c r="A866" t="inlineStr">
         <is>
-          <t>6f87f94b95e7ef0a0100755f8a055936</t>
+          <t>d55bd1e792b56a9b37cab720e6748928</t>
         </is>
       </c>
       <c r="B866" t="inlineStr">
         <is>
-          <t>Peprilus triacanthus</t>
+          <t>Scophthalmus aquosus</t>
         </is>
       </c>
       <c r="C866" t="inlineStr">
         <is>
-          <t>American butterfish</t>
+          <t>Windowpane flounder</t>
         </is>
       </c>
       <c r="D866" t="inlineStr">
@@ -24612,17 +24612,17 @@
     <row r="867">
       <c r="A867" t="inlineStr">
         <is>
-          <t>d55bd1e792b56a9b37cab720e6748928</t>
+          <t>6f87f94b95e7ef0a0100755f8a055936</t>
         </is>
       </c>
       <c r="B867" t="inlineStr">
         <is>
-          <t>Scophthalmus aquosus</t>
+          <t>Peprilus triacanthus</t>
         </is>
       </c>
       <c r="C867" t="inlineStr">
         <is>
-          <t>Windowpane flounder</t>
+          <t>American butterfish</t>
         </is>
       </c>
       <c r="D867" t="inlineStr">
@@ -24640,22 +24640,22 @@
     <row r="868">
       <c r="A868" t="inlineStr">
         <is>
-          <t>5e08caf5fa5e0bfa7e3db058103c1268</t>
+          <t>d8c1357ed6db63f1592172bb927b4b76</t>
         </is>
       </c>
       <c r="B868" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C868" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D868" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E868">
@@ -24668,22 +24668,22 @@
     <row r="869">
       <c r="A869" t="inlineStr">
         <is>
-          <t>d8c1357ed6db63f1592172bb927b4b76</t>
+          <t>5e08caf5fa5e0bfa7e3db058103c1268</t>
         </is>
       </c>
       <c r="B869" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C869" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D869" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E869">
@@ -24780,22 +24780,22 @@
     <row r="873">
       <c r="A873" t="inlineStr">
         <is>
-          <t>ffce0d3f4e4610b271a490f081984407</t>
+          <t>31e6c719fd23f02c12eefc6a51ce2076</t>
         </is>
       </c>
       <c r="B873" t="inlineStr">
         <is>
-          <t>Aythya sp</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C873" t="inlineStr">
         <is>
-          <t>Duck sp</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D873" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E873">
@@ -24808,22 +24808,22 @@
     <row r="874">
       <c r="A874" t="inlineStr">
         <is>
-          <t>31e6c719fd23f02c12eefc6a51ce2076</t>
+          <t>ffce0d3f4e4610b271a490f081984407</t>
         </is>
       </c>
       <c r="B874" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>Aythya sp</t>
         </is>
       </c>
       <c r="C874" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>Duck sp</t>
         </is>
       </c>
       <c r="D874" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E874">
@@ -24892,17 +24892,17 @@
     <row r="877">
       <c r="A877" t="inlineStr">
         <is>
-          <t>25546baa5802e7d9f399a082226768a1</t>
+          <t>1b8389afa98a9962df0c11cc8f97202f</t>
         </is>
       </c>
       <c r="B877" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Urophycis sp</t>
         </is>
       </c>
       <c r="C877" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Red White or Spotted hake</t>
         </is>
       </c>
       <c r="D877" t="inlineStr">
@@ -24920,17 +24920,17 @@
     <row r="878">
       <c r="A878" t="inlineStr">
         <is>
-          <t>1b8389afa98a9962df0c11cc8f97202f</t>
+          <t>25546baa5802e7d9f399a082226768a1</t>
         </is>
       </c>
       <c r="B878" t="inlineStr">
         <is>
-          <t>Urophycis sp</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C878" t="inlineStr">
         <is>
-          <t>Red White or Spotted hake</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D878" t="inlineStr">
@@ -25088,17 +25088,17 @@
     <row r="884">
       <c r="A884" t="inlineStr">
         <is>
-          <t>b8d21918afc6bb5fff719b0c635988b4</t>
+          <t>c1bcc5192d3378e79247e21e8b017069</t>
         </is>
       </c>
       <c r="B884" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Merluccius bilinearis</t>
         </is>
       </c>
       <c r="C884" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Silver hake</t>
         </is>
       </c>
       <c r="D884" t="inlineStr">
@@ -25116,17 +25116,17 @@
     <row r="885">
       <c r="A885" t="inlineStr">
         <is>
-          <t>c1bcc5192d3378e79247e21e8b017069</t>
+          <t>b8d21918afc6bb5fff719b0c635988b4</t>
         </is>
       </c>
       <c r="B885" t="inlineStr">
         <is>
-          <t>Merluccius bilinearis</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C885" t="inlineStr">
         <is>
-          <t>Silver hake</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D885" t="inlineStr">
@@ -25200,22 +25200,22 @@
     <row r="888">
       <c r="A888" t="inlineStr">
         <is>
-          <t>d9230df8d86f06db743d276062a38258</t>
+          <t>40f3675d8b544f218a1bc891019b87c4</t>
         </is>
       </c>
       <c r="B888" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C888" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D888" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E888">
@@ -25256,22 +25256,22 @@
     <row r="890">
       <c r="A890" t="inlineStr">
         <is>
-          <t>40f3675d8b544f218a1bc891019b87c4</t>
+          <t>23f958c05ceb0fb59247b66e24acf584</t>
         </is>
       </c>
       <c r="B890" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C890" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D890" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E890">
@@ -25284,22 +25284,22 @@
     <row r="891">
       <c r="A891" t="inlineStr">
         <is>
-          <t>23f958c05ceb0fb59247b66e24acf584</t>
+          <t>d9230df8d86f06db743d276062a38258</t>
         </is>
       </c>
       <c r="B891" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C891" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D891" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E891">
@@ -25536,22 +25536,22 @@
     <row r="900">
       <c r="A900" t="inlineStr">
         <is>
-          <t>6c88f34060d19d056a22aba44d08fa91</t>
+          <t>1533469db84e906a7d07208d202f0b61</t>
         </is>
       </c>
       <c r="B900" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C900" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D900" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E900">
@@ -25564,17 +25564,17 @@
     <row r="901">
       <c r="A901" t="inlineStr">
         <is>
-          <t>23069cba8195d27fbd56256ca0cde80d</t>
+          <t>6c88f34060d19d056a22aba44d08fa91</t>
         </is>
       </c>
       <c r="B901" t="inlineStr">
         <is>
-          <t>Urophycis sp</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C901" t="inlineStr">
         <is>
-          <t>Red White or Spotted hake</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D901" t="inlineStr">
@@ -25592,22 +25592,22 @@
     <row r="902">
       <c r="A902" t="inlineStr">
         <is>
-          <t>1533469db84e906a7d07208d202f0b61</t>
+          <t>d42c8e8887fabf5e8910f3522eff97c3</t>
         </is>
       </c>
       <c r="B902" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Apeltes quadracus</t>
         </is>
       </c>
       <c r="C902" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Fourspine stickleback</t>
         </is>
       </c>
       <c r="D902" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E902">
@@ -25620,17 +25620,17 @@
     <row r="903">
       <c r="A903" t="inlineStr">
         <is>
-          <t>d42c8e8887fabf5e8910f3522eff97c3</t>
+          <t>23069cba8195d27fbd56256ca0cde80d</t>
         </is>
       </c>
       <c r="B903" t="inlineStr">
         <is>
-          <t>Apeltes quadracus</t>
+          <t>Urophycis sp</t>
         </is>
       </c>
       <c r="C903" t="inlineStr">
         <is>
-          <t>Fourspine stickleback</t>
+          <t>Red White or Spotted hake</t>
         </is>
       </c>
       <c r="D903" t="inlineStr">
@@ -25704,17 +25704,17 @@
     <row r="906">
       <c r="A906" t="inlineStr">
         <is>
-          <t>7cd246298682195e7bf83191f28b7bce</t>
+          <t>52ee96ff6a3c8630f165634002298b99</t>
         </is>
       </c>
       <c r="B906" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Thunnus sp</t>
         </is>
       </c>
       <c r="C906" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Tuna sp</t>
         </is>
       </c>
       <c r="D906" t="inlineStr">
@@ -25732,17 +25732,17 @@
     <row r="907">
       <c r="A907" t="inlineStr">
         <is>
-          <t>52ee96ff6a3c8630f165634002298b99</t>
+          <t>7cd246298682195e7bf83191f28b7bce</t>
         </is>
       </c>
       <c r="B907" t="inlineStr">
         <is>
-          <t>Thunnus sp</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C907" t="inlineStr">
         <is>
-          <t>Tuna sp</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D907" t="inlineStr">
@@ -25760,22 +25760,22 @@
     <row r="908">
       <c r="A908" t="inlineStr">
         <is>
-          <t>fac9357fd7f70206aa72970682f55c7e</t>
+          <t>3d7a7af6852a30194df4c348152dae39</t>
         </is>
       </c>
       <c r="B908" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C908" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D908" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E908">
@@ -25788,22 +25788,22 @@
     <row r="909">
       <c r="A909" t="inlineStr">
         <is>
-          <t>3d7a7af6852a30194df4c348152dae39</t>
+          <t>fac9357fd7f70206aa72970682f55c7e</t>
         </is>
       </c>
       <c r="B909" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C909" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D909" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E909">
@@ -25900,22 +25900,22 @@
     <row r="913">
       <c r="A913" t="inlineStr">
         <is>
-          <t>f5ea7050f3d2bbeb76e077d6fcc785c2</t>
+          <t>7fcfdb27ab75b7670300c22f2d4387ba</t>
         </is>
       </c>
       <c r="B913" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Balaenoptera acutorostrata</t>
         </is>
       </c>
       <c r="C913" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Minke whale</t>
         </is>
       </c>
       <c r="D913" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Marine Mammal</t>
         </is>
       </c>
       <c r="E913">
@@ -25928,17 +25928,17 @@
     <row r="914">
       <c r="A914" t="inlineStr">
         <is>
-          <t>9068e5289a20153e5842cd9d2f9a03b1</t>
+          <t>f5ea7050f3d2bbeb76e077d6fcc785c2</t>
         </is>
       </c>
       <c r="B914" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C914" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D914" t="inlineStr">
@@ -25956,22 +25956,22 @@
     <row r="915">
       <c r="A915" t="inlineStr">
         <is>
-          <t>7fcfdb27ab75b7670300c22f2d4387ba</t>
+          <t>9068e5289a20153e5842cd9d2f9a03b1</t>
         </is>
       </c>
       <c r="B915" t="inlineStr">
         <is>
-          <t>Balaenoptera acutorostrata</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C915" t="inlineStr">
         <is>
-          <t>Minke whale</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D915" t="inlineStr">
         <is>
-          <t>Marine Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E915">
@@ -26068,22 +26068,22 @@
     <row r="919">
       <c r="A919" t="inlineStr">
         <is>
-          <t>c9f51b93de604283020cc9565da2a070</t>
+          <t>89b90c8e5c2458f13f32aa12d457de3d</t>
         </is>
       </c>
       <c r="B919" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Morone saxatilis</t>
         </is>
       </c>
       <c r="C919" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Striped bass</t>
         </is>
       </c>
       <c r="D919" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E919">
@@ -26096,22 +26096,22 @@
     <row r="920">
       <c r="A920" t="inlineStr">
         <is>
-          <t>89b90c8e5c2458f13f32aa12d457de3d</t>
+          <t>c9f51b93de604283020cc9565da2a070</t>
         </is>
       </c>
       <c r="B920" t="inlineStr">
         <is>
-          <t>Morone saxatilis</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C920" t="inlineStr">
         <is>
-          <t>Striped bass</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D920" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E920">
@@ -26208,22 +26208,22 @@
     <row r="924">
       <c r="A924" t="inlineStr">
         <is>
-          <t>a00f5f90120df6b2fff4718c10d12e44</t>
+          <t>50d208d4a622d86c9c17c4fdf9fd4504</t>
         </is>
       </c>
       <c r="B924" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C924" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D924" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E924">
@@ -26236,22 +26236,22 @@
     <row r="925">
       <c r="A925" t="inlineStr">
         <is>
-          <t>50d208d4a622d86c9c17c4fdf9fd4504</t>
+          <t>a00f5f90120df6b2fff4718c10d12e44</t>
         </is>
       </c>
       <c r="B925" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C925" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D925" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E925">
@@ -26460,22 +26460,22 @@
     <row r="933">
       <c r="A933" t="inlineStr">
         <is>
-          <t>0c567e070c2b3453ed6f6f54d9b17657</t>
+          <t>e15783c6c85ffc4f4d3685211ccb9d41</t>
         </is>
       </c>
       <c r="B933" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C933" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D933" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E933">
@@ -26516,22 +26516,22 @@
     <row r="935">
       <c r="A935" t="inlineStr">
         <is>
-          <t>e15783c6c85ffc4f4d3685211ccb9d41</t>
+          <t>0c567e070c2b3453ed6f6f54d9b17657</t>
         </is>
       </c>
       <c r="B935" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C935" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D935" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E935">
@@ -26600,22 +26600,22 @@
     <row r="938">
       <c r="A938" t="inlineStr">
         <is>
-          <t>edbebd208f2e81f3c2327de07a39c476</t>
+          <t>f356c3118beda9519f9a1de3d65b1860</t>
         </is>
       </c>
       <c r="B938" t="inlineStr">
         <is>
-          <t>Leucoraja ocellata or erinacea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C938" t="inlineStr">
         <is>
-          <t>Winter skate or Little skate</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D938" t="inlineStr">
         <is>
-          <t>Elasmobranch</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E938">
@@ -26628,22 +26628,22 @@
     <row r="939">
       <c r="A939" t="inlineStr">
         <is>
-          <t>2d0e9e931c9856d1f73a727500c6a755</t>
+          <t>edbebd208f2e81f3c2327de07a39c476</t>
         </is>
       </c>
       <c r="B939" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Leucoraja ocellata or erinacea</t>
         </is>
       </c>
       <c r="C939" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Winter skate or Little skate</t>
         </is>
       </c>
       <c r="D939" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Elasmobranch</t>
         </is>
       </c>
       <c r="E939">
@@ -26656,22 +26656,22 @@
     <row r="940">
       <c r="A940" t="inlineStr">
         <is>
-          <t>f356c3118beda9519f9a1de3d65b1860</t>
+          <t>2d0e9e931c9856d1f73a727500c6a755</t>
         </is>
       </c>
       <c r="B940" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C940" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D940" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E940">
@@ -26712,22 +26712,22 @@
     <row r="942">
       <c r="A942" t="inlineStr">
         <is>
-          <t>5659308d15f1c66a7cd077b63ca73cb0</t>
+          <t>9203da7049ed5a29617283658d2dfaea</t>
         </is>
       </c>
       <c r="B942" t="inlineStr">
         <is>
-          <t>Delphinus delphis</t>
+          <t>Hippoglossina oblonga</t>
         </is>
       </c>
       <c r="C942" t="inlineStr">
         <is>
-          <t>Shortbeaked common dolphin</t>
+          <t>Fourspot flounder</t>
         </is>
       </c>
       <c r="D942" t="inlineStr">
         <is>
-          <t>Marine Mammal</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E942">
@@ -26740,22 +26740,22 @@
     <row r="943">
       <c r="A943" t="inlineStr">
         <is>
-          <t>9203da7049ed5a29617283658d2dfaea</t>
+          <t>5659308d15f1c66a7cd077b63ca73cb0</t>
         </is>
       </c>
       <c r="B943" t="inlineStr">
         <is>
-          <t>Hippoglossina oblonga</t>
+          <t>Delphinus delphis</t>
         </is>
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>Fourspot flounder</t>
+          <t>Shortbeaked common dolphin</t>
         </is>
       </c>
       <c r="D943" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Marine Mammal</t>
         </is>
       </c>
       <c r="E943">
@@ -26936,22 +26936,22 @@
     <row r="950">
       <c r="A950" t="inlineStr">
         <is>
-          <t>df173b369dc421debeb7bf75520533a5</t>
+          <t>27e6e5f3098de15e1ae9c0959b8ca7d5</t>
         </is>
       </c>
       <c r="B950" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Leucoraja ocellata or erinacea</t>
         </is>
       </c>
       <c r="C950" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Winter skate or Little skate</t>
         </is>
       </c>
       <c r="D950" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Elasmobranch</t>
         </is>
       </c>
       <c r="E950">
@@ -26964,22 +26964,22 @@
     <row r="951">
       <c r="A951" t="inlineStr">
         <is>
-          <t>27e6e5f3098de15e1ae9c0959b8ca7d5</t>
+          <t>df173b369dc421debeb7bf75520533a5</t>
         </is>
       </c>
       <c r="B951" t="inlineStr">
         <is>
-          <t>Leucoraja ocellata or erinacea</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C951" t="inlineStr">
         <is>
-          <t>Winter skate or Little skate</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D951" t="inlineStr">
         <is>
-          <t>Elasmobranch</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E951">
@@ -27020,7 +27020,7 @@
     <row r="953">
       <c r="A953" t="inlineStr">
         <is>
-          <t>d29e6d165e68c4dffb24b1a7d8a27895</t>
+          <t>da8a1934028bb5d7e98dadfe2156a9ea</t>
         </is>
       </c>
       <c r="B953" t="inlineStr">
@@ -27048,7 +27048,7 @@
     <row r="954">
       <c r="A954" t="inlineStr">
         <is>
-          <t>da8a1934028bb5d7e98dadfe2156a9ea</t>
+          <t>d29e6d165e68c4dffb24b1a7d8a27895</t>
         </is>
       </c>
       <c r="B954" t="inlineStr">
@@ -27076,22 +27076,22 @@
     <row r="955">
       <c r="A955" t="inlineStr">
         <is>
-          <t>cd36d419b8e7afc4b6ca44afcc1ece36</t>
+          <t>956f120f6a3dc7feb168dcfaa16c3246</t>
         </is>
       </c>
       <c r="B955" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C955" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D955" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E955">
@@ -27104,22 +27104,22 @@
     <row r="956">
       <c r="A956" t="inlineStr">
         <is>
-          <t>956f120f6a3dc7feb168dcfaa16c3246</t>
+          <t>cd36d419b8e7afc4b6ca44afcc1ece36</t>
         </is>
       </c>
       <c r="B956" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C956" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D956" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E956">
@@ -27160,22 +27160,22 @@
     <row r="958">
       <c r="A958" t="inlineStr">
         <is>
-          <t>98b08e88d8eb2702953318f6566401b8</t>
+          <t>fdecfd64abe5eab77910f8df76479fd8</t>
         </is>
       </c>
       <c r="B958" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C958" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D958" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E958">
@@ -27188,22 +27188,22 @@
     <row r="959">
       <c r="A959" t="inlineStr">
         <is>
-          <t>fdecfd64abe5eab77910f8df76479fd8</t>
+          <t>98b08e88d8eb2702953318f6566401b8</t>
         </is>
       </c>
       <c r="B959" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C959" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D959" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E959">
@@ -27244,22 +27244,22 @@
     <row r="961">
       <c r="A961" t="inlineStr">
         <is>
-          <t>d7caf7e9717e18578516f34f5e324b53</t>
+          <t>05728ce3d6a09550ee64c2f76f3a3676</t>
         </is>
       </c>
       <c r="B961" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Cottidae sp</t>
         </is>
       </c>
       <c r="C961" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Sculpins</t>
         </is>
       </c>
       <c r="D961" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E961">
@@ -27272,22 +27272,22 @@
     <row r="962">
       <c r="A962" t="inlineStr">
         <is>
-          <t>01fddebb1fe784a669f47c356f1e788b</t>
+          <t>d7caf7e9717e18578516f34f5e324b53</t>
         </is>
       </c>
       <c r="B962" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C962" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D962" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E962">
@@ -27300,17 +27300,17 @@
     <row r="963">
       <c r="A963" t="inlineStr">
         <is>
-          <t>05728ce3d6a09550ee64c2f76f3a3676</t>
+          <t>01fddebb1fe784a669f47c356f1e788b</t>
         </is>
       </c>
       <c r="B963" t="inlineStr">
         <is>
-          <t>Cottidae sp</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C963" t="inlineStr">
         <is>
-          <t>Sculpins</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D963" t="inlineStr">
@@ -27328,22 +27328,22 @@
     <row r="964">
       <c r="A964" t="inlineStr">
         <is>
-          <t>8c4afbf7ea36d37b1d6731dafc689040</t>
+          <t>ac63f4f787ba6627ddba9d59b10ecab2</t>
         </is>
       </c>
       <c r="B964" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C964" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D964" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E964">
@@ -27356,22 +27356,22 @@
     <row r="965">
       <c r="A965" t="inlineStr">
         <is>
-          <t>ac63f4f787ba6627ddba9d59b10ecab2</t>
+          <t>8c4afbf7ea36d37b1d6731dafc689040</t>
         </is>
       </c>
       <c r="B965" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C965" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D965" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E965">
@@ -27440,22 +27440,22 @@
     <row r="968">
       <c r="A968" t="inlineStr">
         <is>
-          <t>4d780165eff0994baade3111bba9f754</t>
+          <t>9bc7899e8fc369bed86e93ca8c72e359</t>
         </is>
       </c>
       <c r="B968" t="inlineStr">
         <is>
-          <t>Lamna nasus</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C968" t="inlineStr">
         <is>
-          <t>Porbeagle shark</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D968" t="inlineStr">
         <is>
-          <t>Elasmobranch</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E968">
@@ -27468,22 +27468,22 @@
     <row r="969">
       <c r="A969" t="inlineStr">
         <is>
-          <t>b78bf43755a4a2bf34300fcfeda8c15c</t>
+          <t>4d780165eff0994baade3111bba9f754</t>
         </is>
       </c>
       <c r="B969" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Lamna nasus</t>
         </is>
       </c>
       <c r="C969" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Porbeagle shark</t>
         </is>
       </c>
       <c r="D969" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Elasmobranch</t>
         </is>
       </c>
       <c r="E969">
@@ -27496,22 +27496,22 @@
     <row r="970">
       <c r="A970" t="inlineStr">
         <is>
-          <t>9bc7899e8fc369bed86e93ca8c72e359</t>
+          <t>b78bf43755a4a2bf34300fcfeda8c15c</t>
         </is>
       </c>
       <c r="B970" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C970" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D970" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E970">
@@ -27608,17 +27608,17 @@
     <row r="974">
       <c r="A974" t="inlineStr">
         <is>
-          <t>9682be6fbd648d7d3795747d603f3f65</t>
+          <t>acbe17050ee6914bd81d372dd39bcba9</t>
         </is>
       </c>
       <c r="B974" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Clupeidae sp</t>
         </is>
       </c>
       <c r="C974" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Atlantic menhaden or River herrings</t>
         </is>
       </c>
       <c r="D974" t="inlineStr">
@@ -27636,17 +27636,17 @@
     <row r="975">
       <c r="A975" t="inlineStr">
         <is>
-          <t>acbe17050ee6914bd81d372dd39bcba9</t>
+          <t>9682be6fbd648d7d3795747d603f3f65</t>
         </is>
       </c>
       <c r="B975" t="inlineStr">
         <is>
-          <t>Clupeidae sp</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C975" t="inlineStr">
         <is>
-          <t>Atlantic menhaden or River herrings</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D975" t="inlineStr">
@@ -27664,22 +27664,22 @@
     <row r="976">
       <c r="A976" t="inlineStr">
         <is>
-          <t>309d79f35545611f523a658f074d1d80</t>
+          <t>8b80e1b346f690fdb5eb745140c9b780</t>
         </is>
       </c>
       <c r="B976" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Larus delawarensis</t>
         </is>
       </c>
       <c r="C976" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Ring billed gull</t>
         </is>
       </c>
       <c r="D976" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E976">
@@ -27692,22 +27692,22 @@
     <row r="977">
       <c r="A977" t="inlineStr">
         <is>
-          <t>8b80e1b346f690fdb5eb745140c9b780</t>
+          <t>309d79f35545611f523a658f074d1d80</t>
         </is>
       </c>
       <c r="B977" t="inlineStr">
         <is>
-          <t>Larus delawarensis</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C977" t="inlineStr">
         <is>
-          <t>Ring billed gull</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D977" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E977">
@@ -27776,17 +27776,17 @@
     <row r="980">
       <c r="A980" t="inlineStr">
         <is>
-          <t>60e2a4e2a76331e202a75c03a297125d</t>
+          <t>94385478d7e7e954f9f6e1bddac1171c</t>
         </is>
       </c>
       <c r="B980" t="inlineStr">
         <is>
-          <t>Hippoglossina oblonga</t>
+          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
         </is>
       </c>
       <c r="C980" t="inlineStr">
         <is>
-          <t>Fourspot flounder</t>
+          <t>Winter or Yellowtail flounder</t>
         </is>
       </c>
       <c r="D980" t="inlineStr">
@@ -27804,17 +27804,17 @@
     <row r="981">
       <c r="A981" t="inlineStr">
         <is>
-          <t>94385478d7e7e954f9f6e1bddac1171c</t>
+          <t>60e2a4e2a76331e202a75c03a297125d</t>
         </is>
       </c>
       <c r="B981" t="inlineStr">
         <is>
-          <t>Pseudopleuronectes americanus or Myzopsetta ferruginea</t>
+          <t>Hippoglossina oblonga</t>
         </is>
       </c>
       <c r="C981" t="inlineStr">
         <is>
-          <t>Winter or Yellowtail flounder</t>
+          <t>Fourspot flounder</t>
         </is>
       </c>
       <c r="D981" t="inlineStr">
@@ -27832,22 +27832,22 @@
     <row r="982">
       <c r="A982" t="inlineStr">
         <is>
-          <t>ac1550894d847e7287a0295f64024935</t>
+          <t>ae13360e6aef27d5511183d08158cfcb</t>
         </is>
       </c>
       <c r="B982" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Clangula hyemalis or other Anatidae sp</t>
         </is>
       </c>
       <c r="C982" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Long tailed duck or other ducks</t>
         </is>
       </c>
       <c r="D982" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E982">
@@ -27860,22 +27860,22 @@
     <row r="983">
       <c r="A983" t="inlineStr">
         <is>
-          <t>ae13360e6aef27d5511183d08158cfcb</t>
+          <t>ac1550894d847e7287a0295f64024935</t>
         </is>
       </c>
       <c r="B983" t="inlineStr">
         <is>
-          <t>Clangula hyemalis or other Anatidae sp</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C983" t="inlineStr">
         <is>
-          <t>Long tailed duck or other ducks</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D983" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E983">
@@ -27888,22 +27888,22 @@
     <row r="984">
       <c r="A984" t="inlineStr">
         <is>
-          <t>13bed3b63b5f71f7671c2ce1f244f283</t>
+          <t>f6bf0cd9dd39f654750c9915533c6274</t>
         </is>
       </c>
       <c r="B984" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C984" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D984" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E984">
@@ -27944,22 +27944,22 @@
     <row r="986">
       <c r="A986" t="inlineStr">
         <is>
-          <t>f6bf0cd9dd39f654750c9915533c6274</t>
+          <t>13bed3b63b5f71f7671c2ce1f244f283</t>
         </is>
       </c>
       <c r="B986" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C986" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D986" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E986">
@@ -28028,17 +28028,17 @@
     <row r="989">
       <c r="A989" t="inlineStr">
         <is>
-          <t>3a862926c908e692a6d38ebff9c4638d</t>
+          <t>ef3c720fe10077a72d4b01803b49f7ee</t>
         </is>
       </c>
       <c r="B989" t="inlineStr">
         <is>
-          <t>Stenotomus chrysops</t>
+          <t>Fundulus heteroclitus</t>
         </is>
       </c>
       <c r="C989" t="inlineStr">
         <is>
-          <t>Scup</t>
+          <t>Mummichog</t>
         </is>
       </c>
       <c r="D989" t="inlineStr">
@@ -28084,17 +28084,17 @@
     <row r="991">
       <c r="A991" t="inlineStr">
         <is>
-          <t>ef3c720fe10077a72d4b01803b49f7ee</t>
+          <t>3a862926c908e692a6d38ebff9c4638d</t>
         </is>
       </c>
       <c r="B991" t="inlineStr">
         <is>
-          <t>Fundulus heteroclitus</t>
+          <t>Stenotomus chrysops</t>
         </is>
       </c>
       <c r="C991" t="inlineStr">
         <is>
-          <t>Mummichog</t>
+          <t>Scup</t>
         </is>
       </c>
       <c r="D991" t="inlineStr">
@@ -28168,17 +28168,17 @@
     <row r="994">
       <c r="A994" t="inlineStr">
         <is>
-          <t>f4a36133436b726d606a22bf90e19435</t>
+          <t>2a0006eeeda0f4a9cd4a92fd42fd1f91</t>
         </is>
       </c>
       <c r="B994" t="inlineStr">
         <is>
-          <t>Menidia beryllina</t>
+          <t>Merluccius bilinearis</t>
         </is>
       </c>
       <c r="C994" t="inlineStr">
         <is>
-          <t>Inland silverside</t>
+          <t>Silver hake</t>
         </is>
       </c>
       <c r="D994" t="inlineStr">
@@ -28196,17 +28196,17 @@
     <row r="995">
       <c r="A995" t="inlineStr">
         <is>
-          <t>2a0006eeeda0f4a9cd4a92fd42fd1f91</t>
+          <t>f4a36133436b726d606a22bf90e19435</t>
         </is>
       </c>
       <c r="B995" t="inlineStr">
         <is>
-          <t>Merluccius bilinearis</t>
+          <t>Menidia beryllina</t>
         </is>
       </c>
       <c r="C995" t="inlineStr">
         <is>
-          <t>Silver hake</t>
+          <t>Inland silverside</t>
         </is>
       </c>
       <c r="D995" t="inlineStr">
@@ -28252,7 +28252,7 @@
     <row r="997">
       <c r="A997" t="inlineStr">
         <is>
-          <t>33a60f64837ff0cf0d71c46d2af17273</t>
+          <t>7a59e4544d999c3fd8724d3a77ef1aad</t>
         </is>
       </c>
       <c r="B997" t="inlineStr">
@@ -28280,7 +28280,7 @@
     <row r="998">
       <c r="A998" t="inlineStr">
         <is>
-          <t>7a59e4544d999c3fd8724d3a77ef1aad</t>
+          <t>33a60f64837ff0cf0d71c46d2af17273</t>
         </is>
       </c>
       <c r="B998" t="inlineStr">
@@ -28532,22 +28532,22 @@
     <row r="1007">
       <c r="A1007" t="inlineStr">
         <is>
-          <t>161473b17b1d75bdf07e9d19c77c2edb</t>
+          <t>0db2a1413e76c1894ff2dfd34d54aa25</t>
         </is>
       </c>
       <c r="B1007" t="inlineStr">
         <is>
-          <t>Ammodytes dubius</t>
+          <t>Squalus acanthias</t>
         </is>
       </c>
       <c r="C1007" t="inlineStr">
         <is>
-          <t>Northern sand lance</t>
+          <t>Spiny dogfish</t>
         </is>
       </c>
       <c r="D1007" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Elasmobranch</t>
         </is>
       </c>
       <c r="E1007">
@@ -28560,22 +28560,22 @@
     <row r="1008">
       <c r="A1008" t="inlineStr">
         <is>
-          <t>0db2a1413e76c1894ff2dfd34d54aa25</t>
+          <t>161473b17b1d75bdf07e9d19c77c2edb</t>
         </is>
       </c>
       <c r="B1008" t="inlineStr">
         <is>
-          <t>Squalus acanthias</t>
+          <t>Ammodytes dubius</t>
         </is>
       </c>
       <c r="C1008" t="inlineStr">
         <is>
-          <t>Spiny dogfish</t>
+          <t>Northern sand lance</t>
         </is>
       </c>
       <c r="D1008" t="inlineStr">
         <is>
-          <t>Elasmobranch</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1008">
@@ -28756,22 +28756,22 @@
     <row r="1015">
       <c r="A1015" t="inlineStr">
         <is>
-          <t>68c925ef918309f7445043a45c0dbc97</t>
+          <t>77b7e8fcc6ae79f4a5c42418b68af534</t>
         </is>
       </c>
       <c r="B1015" t="inlineStr">
         <is>
-          <t>Menidia menidia</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1015" t="inlineStr">
         <is>
-          <t>Atlantic silverside</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1015" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1015">
@@ -28784,22 +28784,22 @@
     <row r="1016">
       <c r="A1016" t="inlineStr">
         <is>
-          <t>77b7e8fcc6ae79f4a5c42418b68af534</t>
+          <t>68c925ef918309f7445043a45c0dbc97</t>
         </is>
       </c>
       <c r="B1016" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Menidia menidia</t>
         </is>
       </c>
       <c r="C1016" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Atlantic silverside</t>
         </is>
       </c>
       <c r="D1016" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1016">
@@ -29092,22 +29092,22 @@
     <row r="1027">
       <c r="A1027" t="inlineStr">
         <is>
-          <t>989013af2395aea06e80451cf08681fa</t>
+          <t>3d7ba42c182ded4417ed587f3e448c10</t>
         </is>
       </c>
       <c r="B1027" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Urophycis sp</t>
         </is>
       </c>
       <c r="C1027" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Red White or Spotted hake</t>
         </is>
       </c>
       <c r="D1027" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1027">
@@ -29120,22 +29120,22 @@
     <row r="1028">
       <c r="A1028" t="inlineStr">
         <is>
-          <t>3d7ba42c182ded4417ed587f3e448c10</t>
+          <t>989013af2395aea06e80451cf08681fa</t>
         </is>
       </c>
       <c r="B1028" t="inlineStr">
         <is>
-          <t>Urophycis sp</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C1028" t="inlineStr">
         <is>
-          <t>Red White or Spotted hake</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D1028" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E1028">
@@ -29176,7 +29176,7 @@
     <row r="1030">
       <c r="A1030" t="inlineStr">
         <is>
-          <t>5face5fc033796391746e552a0ec24cb</t>
+          <t>2730e679d76db8fb905071699b5b5902</t>
         </is>
       </c>
       <c r="B1030" t="inlineStr">
@@ -29232,7 +29232,7 @@
     <row r="1032">
       <c r="A1032" t="inlineStr">
         <is>
-          <t>2730e679d76db8fb905071699b5b5902</t>
+          <t>5face5fc033796391746e552a0ec24cb</t>
         </is>
       </c>
       <c r="B1032" t="inlineStr">
@@ -29288,22 +29288,22 @@
     <row r="1034">
       <c r="A1034" t="inlineStr">
         <is>
-          <t>44059a4da86405acd7eaaf549b5f4b90</t>
+          <t>4cf525c05249ccde63f0b41a9f260c95</t>
         </is>
       </c>
       <c r="B1034" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Trinectes maculatus</t>
         </is>
       </c>
       <c r="C1034" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Hogchoker</t>
         </is>
       </c>
       <c r="D1034" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1034">
@@ -29316,22 +29316,22 @@
     <row r="1035">
       <c r="A1035" t="inlineStr">
         <is>
-          <t>4cf525c05249ccde63f0b41a9f260c95</t>
+          <t>44059a4da86405acd7eaaf549b5f4b90</t>
         </is>
       </c>
       <c r="B1035" t="inlineStr">
         <is>
-          <t>Trinectes maculatus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1035" t="inlineStr">
         <is>
-          <t>Hogchoker</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1035" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1035">
@@ -29456,22 +29456,22 @@
     <row r="1040">
       <c r="A1040" t="inlineStr">
         <is>
-          <t>05f0b67ae73a314a3e10009adc99f258</t>
+          <t>16de09dbce953f9fed0846f679270d3a</t>
         </is>
       </c>
       <c r="B1040" t="inlineStr">
         <is>
-          <t>Fundulus majalis</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C1040" t="inlineStr">
         <is>
-          <t>Striped killifish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D1040" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E1040">
@@ -29484,22 +29484,22 @@
     <row r="1041">
       <c r="A1041" t="inlineStr">
         <is>
-          <t>16de09dbce953f9fed0846f679270d3a</t>
+          <t>05f0b67ae73a314a3e10009adc99f258</t>
         </is>
       </c>
       <c r="B1041" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Fundulus majalis</t>
         </is>
       </c>
       <c r="C1041" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Striped killifish</t>
         </is>
       </c>
       <c r="D1041" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1041">
@@ -29624,7 +29624,7 @@
     <row r="1046">
       <c r="A1046" t="inlineStr">
         <is>
-          <t>b1b35b12910432aa298c54ecdce4a8f7</t>
+          <t>f332d5c9e8a41b8bca91750fd8a1cfb6</t>
         </is>
       </c>
       <c r="B1046" t="inlineStr">
@@ -29652,22 +29652,22 @@
     <row r="1047">
       <c r="A1047" t="inlineStr">
         <is>
-          <t>b5341d0559b4434a236acd7e900bd99f</t>
+          <t>c1fba42e7b2939f4c3fb1c6f9175d29d</t>
         </is>
       </c>
       <c r="B1047" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1047" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1047" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1047">
@@ -29680,7 +29680,7 @@
     <row r="1048">
       <c r="A1048" t="inlineStr">
         <is>
-          <t>fb3f006b207ccff926d655d24e1ef99b</t>
+          <t>b1b35b12910432aa298c54ecdce4a8f7</t>
         </is>
       </c>
       <c r="B1048" t="inlineStr">
@@ -29708,22 +29708,22 @@
     <row r="1049">
       <c r="A1049" t="inlineStr">
         <is>
-          <t>c1fba42e7b2939f4c3fb1c6f9175d29d</t>
+          <t>b5341d0559b4434a236acd7e900bd99f</t>
         </is>
       </c>
       <c r="B1049" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C1049" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D1049" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E1049">
@@ -29736,7 +29736,7 @@
     <row r="1050">
       <c r="A1050" t="inlineStr">
         <is>
-          <t>f332d5c9e8a41b8bca91750fd8a1cfb6</t>
+          <t>fb3f006b207ccff926d655d24e1ef99b</t>
         </is>
       </c>
       <c r="B1050" t="inlineStr">
@@ -29792,22 +29792,22 @@
     <row r="1052">
       <c r="A1052" t="inlineStr">
         <is>
-          <t>968ffaa6263a2b507741a95d4d94acc8</t>
+          <t>4abb11778fa0c536622edbb24b7e2a10</t>
         </is>
       </c>
       <c r="B1052" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Centropristis striata</t>
         </is>
       </c>
       <c r="C1052" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Black sea bass</t>
         </is>
       </c>
       <c r="D1052" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1052">
@@ -29820,22 +29820,22 @@
     <row r="1053">
       <c r="A1053" t="inlineStr">
         <is>
-          <t>98c46541b18384d910296f8876423168</t>
+          <t>7dbc53c10ef5a6acd4d8899c653bb8ca</t>
         </is>
       </c>
       <c r="B1053" t="inlineStr">
         <is>
-          <t>Brevoortia tyrannus</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1053" t="inlineStr">
         <is>
-          <t>Atlantic menhaden</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1053" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1053">
@@ -29848,7 +29848,7 @@
     <row r="1054">
       <c r="A1054" t="inlineStr">
         <is>
-          <t>7dbc53c10ef5a6acd4d8899c653bb8ca</t>
+          <t>4ac4a7d11690f2bfa36dde987faf71e6</t>
         </is>
       </c>
       <c r="B1054" t="inlineStr">
@@ -29904,22 +29904,22 @@
     <row r="1056">
       <c r="A1056" t="inlineStr">
         <is>
-          <t>4abb11778fa0c536622edbb24b7e2a10</t>
+          <t>968ffaa6263a2b507741a95d4d94acc8</t>
         </is>
       </c>
       <c r="B1056" t="inlineStr">
         <is>
-          <t>Centropristis striata</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1056" t="inlineStr">
         <is>
-          <t>Black sea bass</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1056" t="inlineStr">
         <is>
-          <t>Teleost Fish</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1056">
@@ -29932,22 +29932,22 @@
     <row r="1057">
       <c r="A1057" t="inlineStr">
         <is>
-          <t>4ac4a7d11690f2bfa36dde987faf71e6</t>
+          <t>98c46541b18384d910296f8876423168</t>
         </is>
       </c>
       <c r="B1057" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Brevoortia tyrannus</t>
         </is>
       </c>
       <c r="C1057" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Atlantic menhaden</t>
         </is>
       </c>
       <c r="D1057" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Teleost Fish</t>
         </is>
       </c>
       <c r="E1057">
@@ -29960,7 +29960,7 @@
     <row r="1058">
       <c r="A1058" t="inlineStr">
         <is>
-          <t>3032263cd6cb95c33a5f0d7d6f3fd683</t>
+          <t>138fe8b6ec8b6e105649f4a8f28e2b97</t>
         </is>
       </c>
       <c r="B1058" t="inlineStr">
@@ -29988,22 +29988,22 @@
     <row r="1059">
       <c r="A1059" t="inlineStr">
         <is>
-          <t>990e5702f47f9a52ee0bbde5c9f0ce1e</t>
+          <t>3a625265e38fe94b2fb31d28a8e9ec2b</t>
         </is>
       </c>
       <c r="B1059" t="inlineStr">
         <is>
-          <t>Ardenna gravis</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1059" t="inlineStr">
         <is>
-          <t>Great Shearwater</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1059" t="inlineStr">
         <is>
-          <t>Bird</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1059">
@@ -30016,22 +30016,22 @@
     <row r="1060">
       <c r="A1060" t="inlineStr">
         <is>
-          <t>149497a0bcff1a347a2658f623aa735d</t>
+          <t>20214d0bb5d29ee990707b92aec89710</t>
         </is>
       </c>
       <c r="B1060" t="inlineStr">
         <is>
-          <t>Homo sapiens</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="C1060" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="D1060" t="inlineStr">
         <is>
-          <t>Human</t>
+          <t>Unassigned</t>
         </is>
       </c>
       <c r="E1060">
@@ -30044,22 +30044,22 @@
     <row r="1061">
       <c r="A1061" t="inlineStr">
         <is>
-          <t>138fe8b6ec8b6e105649f4a8f28e2b97</t>
+          <t>149497a0bcff1a347a2658f623aa735d</t>
         </is>
       </c>
       <c r="B1061" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Homo sapiens</t>
         </is>
       </c>
       <c r="C1061" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="D1061" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Human</t>
         </is>
       </c>
       <c r="E1061">
@@ -30072,7 +30072,7 @@
     <row r="1062">
       <c r="A1062" t="inlineStr">
         <is>
-          <t>3a625265e38fe94b2fb31d28a8e9ec2b</t>
+          <t>2e70f9f98943a06ba097a2f3a028ca98</t>
         </is>
       </c>
       <c r="B1062" t="inlineStr">
@@ -30100,7 +30100,7 @@
     <row r="1063">
       <c r="A1063" t="inlineStr">
         <is>
-          <t>2a2d9a5e1d3b393db0e6adc5d2f901a4</t>
+          <t>3032263cd6cb95c33a5f0d7d6f3fd683</t>
         </is>
       </c>
       <c r="B1063" t="inlineStr">
@@ -30128,22 +30128,22 @@
     <row r="1064">
       <c r="A1064" t="inlineStr">
         <is>
-          <t>8a878e3fc50f02831a3677dbb3eacde2</t>
+          <t>990e5702f47f9a52ee0bbde5c9f0ce1e</t>
         </is>
       </c>
       <c r="B1064" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Ardenna gravis</t>
         </is>
       </c>
       <c r="C1064" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Great Shearwater</t>
         </is>
       </c>
       <c r="D1064" t="inlineStr">
         <is>
-          <t>Unassigned</t>
+          <t>Bird</t>
         </is>
       </c>
       <c r="E1064">
@@ -30156,7 +30156,7 @@
     <row r="1065">
       <c r="A1065" t="inlineStr">
         <is>
-          <t>20214d0bb5d29ee990707b92aec89710</t>
+          <t>2a2d9a5e1d3b393db0e6adc5d2f901a4</t>
         </is>
       </c>
       <c r="B1065" t="inlineStr">
@@ -30184,7 +30184,7 @@
     <row r="1066">
       <c r="A1066" t="inlineStr">
         <is>
-          <t>2e70f9f98943a06ba097a2f3a028ca98</t>
+          <t>8a878e3fc50f02831a3677dbb3eacde2</t>
         </is>
       </c>
       <c r="B1066" t="inlineStr">

</xml_diff>